<commit_message>
fixed text starts with = in chk 11
</commit_message>
<xml_diff>
--- a/Prototype.xlsx
+++ b/Prototype.xlsx
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="1077">
   <si>
     <t>thisdwg</t>
   </si>
@@ -3655,13 +3655,16 @@
     <t>LEGEND DIAGRAM ELEVATION</t>
   </si>
   <si>
-    <t>KST-0220.dwg</t>
-  </si>
-  <si>
     <t>NO in title?</t>
   </si>
   <si>
     <t>xrefsinmodel</t>
+  </si>
+  <si>
+    <t>is view?</t>
+  </si>
+  <si>
+    <t>KSA-1-OV.dwg</t>
   </si>
 </sst>
 </file>
@@ -4444,7 +4447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -4677,6 +4680,8 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6603,8 +6608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GY151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="CN1" workbookViewId="0">
+      <selection activeCell="DF1" sqref="DF1:DF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6685,7 +6690,7 @@
     <col min="107" max="107" width="12.125" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="10.625" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="76.375" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="76.375" style="139" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="10.875" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="11.375" bestFit="1" customWidth="1"/>
     <col min="113" max="114" width="9.125" customWidth="1"/>
@@ -6734,8 +6739,8 @@
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1073</v>
+      <c r="B1" s="2" t="s">
+        <v>1076</v>
       </c>
       <c r="C1" s="67"/>
       <c r="D1" s="74" t="s">
@@ -6924,7 +6929,7 @@
         <v>666</v>
       </c>
       <c r="DE1" s="5"/>
-      <c r="DF1" s="5"/>
+      <c r="DF1" s="164"/>
       <c r="DG1" s="5"/>
       <c r="DH1" s="6"/>
       <c r="DJ1" s="37"/>
@@ -7339,7 +7344,7 @@
       <c r="DE2" s="2">
         <v>0</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DF2" s="138" t="s">
         <v>667</v>
       </c>
       <c r="DG2" s="2" t="s">
@@ -7697,7 +7702,7 @@
       <c r="DE3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF3" s="2" t="s">
+      <c r="DF3" s="138" t="s">
         <v>669</v>
       </c>
       <c r="DG3" s="2" t="s">
@@ -7888,7 +7893,7 @@
       <c r="B4" s="37"/>
       <c r="D4" s="21" t="str">
         <f>thisdwg</f>
-        <v>KST-0220.dwg</v>
+        <v>KSA-1-OV.dwg</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
@@ -8086,7 +8091,7 @@
       <c r="DE4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF4" s="2" t="s">
+      <c r="DF4" s="138" t="s">
         <v>671</v>
       </c>
       <c r="DG4" s="2" t="s">
@@ -8266,7 +8271,7 @@
       <c r="B5" s="37"/>
       <c r="D5" s="22" t="str">
         <f>REPLACE(thisdwg,FIND(".dwg",thisdwg),4,"")</f>
-        <v>KST-0220</v>
+        <v>KSA-1-OV</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="124" t="s">
@@ -8297,7 +8302,7 @@
       </c>
       <c r="X5" s="37" t="str">
         <f>IsLayout</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Y5" s="25"/>
       <c r="Z5" s="37"/>
@@ -8470,7 +8475,7 @@
       <c r="DE5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF5" s="2" t="s">
+      <c r="DF5" s="138" t="s">
         <v>672</v>
       </c>
       <c r="DG5" s="2" t="s">
@@ -8683,7 +8688,7 @@
       </c>
       <c r="G6" s="128" t="str">
         <f>IF(IsLayout="Yes","a layout","a non-layout")</f>
-        <v>a non-layout</v>
+        <v>a layout</v>
       </c>
       <c r="H6" s="129" t="s">
         <v>812</v>
@@ -8699,8 +8704,13 @@
       <c r="L6" s="37"/>
       <c r="M6" s="25"/>
       <c r="N6" s="37"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="37"/>
+      <c r="O6" s="24" t="s">
+        <v>1075</v>
+      </c>
+      <c r="P6" s="37" t="str">
+        <f>IsView</f>
+        <v>Yes</v>
+      </c>
       <c r="Q6" s="37"/>
       <c r="R6" s="37"/>
       <c r="S6" s="37"/>
@@ -8813,7 +8823,7 @@
       </c>
       <c r="CG6" s="37" t="str">
         <f>IsLayout</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="CH6" s="37"/>
       <c r="CI6" s="37"/>
@@ -8870,7 +8880,7 @@
       <c r="DE6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF6" s="2" t="s">
+      <c r="DF6" s="138" t="s">
         <v>673</v>
       </c>
       <c r="DG6" s="2" t="s">
@@ -8918,7 +8928,7 @@
       </c>
       <c r="DY6" s="25" t="str">
         <f>IsLayout</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="DZ6" s="25"/>
       <c r="EA6" s="37"/>
@@ -9201,7 +9211,7 @@
       <c r="DE7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF7" s="2" t="s">
+      <c r="DF7" s="138" t="s">
         <v>674</v>
       </c>
       <c r="DG7" s="2" t="s">
@@ -9360,7 +9370,7 @@
       </c>
       <c r="E8" s="25" t="str">
         <f>MID(thisdwg,3,1)</f>
-        <v>T</v>
+        <v>A</v>
       </c>
       <c r="F8" s="127" t="s">
         <v>815</v>
@@ -9383,7 +9393,7 @@
       </c>
       <c r="P8" s="37" t="str">
         <f>IsLayout</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>
@@ -9400,7 +9410,7 @@
       </c>
       <c r="X8" s="87" t="str">
         <f>IF(IsView="Yes",IF(OR(IsLayout="Yes",IsEnlarged="Yes"),IF(X6="Yes","ok","x"),"na"),"na")</f>
-        <v>na</v>
+        <v>ok</v>
       </c>
       <c r="Y8" s="27"/>
       <c r="Z8" s="37"/>
@@ -9542,7 +9552,7 @@
       <c r="DE8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF8" s="2" t="s">
+      <c r="DF8" s="138" t="s">
         <v>675</v>
       </c>
       <c r="DG8" s="2" t="s">
@@ -9691,7 +9701,7 @@
       </c>
       <c r="G9" s="128" t="str">
         <f>discipline</f>
-        <v xml:space="preserve">Telecommunications </v>
+        <v xml:space="preserve">Architectural </v>
       </c>
       <c r="H9" s="129" t="s">
         <v>818</v>
@@ -9709,7 +9719,7 @@
       </c>
       <c r="P9" s="101" t="str">
         <f>IF(IsLayout="Yes",xrefNameProper,"")</f>
-        <v/>
+        <v>GSA-1-OV</v>
       </c>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
@@ -9856,7 +9866,7 @@
       <c r="DE9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF9" s="2" t="s">
+      <c r="DF9" s="138" t="s">
         <v>676</v>
       </c>
       <c r="DG9" s="2" t="s">
@@ -9998,14 +10008,14 @@
       </c>
       <c r="E10" s="25" t="str">
         <f>MID(thisdwg,5,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="127" t="s">
         <v>819</v>
       </c>
       <c r="G10" s="128" t="str">
         <f>IF(IsLayout="Yes","Layout",series)</f>
-        <v>Diagrams and schematics (e.g. block, ladder, one-line and riser diagrams, PLC Communication), Electrical panel</v>
+        <v>Layout</v>
       </c>
       <c r="H10" s="129"/>
       <c r="I10" s="37"/>
@@ -10177,7 +10187,7 @@
       <c r="DE10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF10" s="2">
+      <c r="DF10" s="138">
         <v>1</v>
       </c>
       <c r="DG10" s="2" t="s">
@@ -10314,15 +10324,15 @@
       </c>
       <c r="E11" s="25" t="str">
         <f>MID(thisdwg,6,1)</f>
-        <v>2</v>
+        <v>-</v>
       </c>
       <c r="F11" s="127" t="str">
         <f>IF(IsLayout="Yes","Level is:","")</f>
-        <v/>
+        <v>Level is:</v>
       </c>
       <c r="G11" s="128" t="str">
         <f>IF(IsLayout="Yes",E27,"")</f>
-        <v/>
+        <v>Level 1 (Ground)</v>
       </c>
       <c r="H11" s="129"/>
       <c r="I11" s="37"/>
@@ -10472,7 +10482,7 @@
       <c r="DE11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF11" s="2" t="s">
+      <c r="DF11" s="138" t="s">
         <v>677</v>
       </c>
       <c r="DG11" s="2" t="s">
@@ -10505,7 +10515,7 @@
       </c>
       <c r="DY11" s="92" t="str">
         <f>IF(IsView="Yes",IF(AND(IsLayout="No",DY7="No"),"na",IF(AND(northarrowok="Yes",OR(IsLayout="Yes",DY7="Yes")),"ok","x")),"na")</f>
-        <v>na</v>
+        <v>x</v>
       </c>
       <c r="DZ11" s="78"/>
       <c r="EA11" s="67"/>
@@ -10614,15 +10624,15 @@
       </c>
       <c r="E12" s="25" t="str">
         <f>MID(thisdwg,7,1)</f>
-        <v>2</v>
+        <v>O</v>
       </c>
       <c r="F12" s="127" t="str">
         <f>IF(IsLayout="Yes","in sector","")</f>
-        <v/>
+        <v>in sector</v>
       </c>
       <c r="G12" s="128" t="str">
         <f>IF(IsLayout="Yes",sector,"")</f>
-        <v/>
+        <v>Overview</v>
       </c>
       <c r="H12" s="129"/>
       <c r="I12" s="37"/>
@@ -10640,7 +10650,7 @@
       </c>
       <c r="P12" s="37" t="str">
         <f>IF(ISERROR(VLOOKUP(xrefNameProper,xrefnames,1,FALSE)),"No",IF(VLOOKUP(xrefNameProper,xrefnames,1,FALSE)=xrefNameProper,"Yes","No"))</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Q12" s="37"/>
       <c r="R12" s="37"/>
@@ -10777,7 +10787,7 @@
       <c r="DE12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF12" s="2" t="s">
+      <c r="DF12" s="138" t="s">
         <v>678</v>
       </c>
       <c r="DG12" s="2" t="s">
@@ -10922,7 +10932,7 @@
       </c>
       <c r="E13" s="25" t="str">
         <f>MID(thisdwg,8,1)</f>
-        <v>0</v>
+        <v>V</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -11074,7 +11084,7 @@
       <c r="DE13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF13" s="2" t="s">
+      <c r="DF13" s="138" t="s">
         <v>679</v>
       </c>
       <c r="DG13" s="2" t="s">
@@ -11230,7 +11240,7 @@
         <v>74</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="M14" s="25" t="str">
         <f>IF(LEN(SUBSTITUTE(Scale,"NO",""))&lt;LEN(Scale),"Yes","No")</f>
@@ -11241,8 +11251,8 @@
         <v>573</v>
       </c>
       <c r="P14" s="71" t="str">
-        <f>IF(IsView="Yes",IF(OR(IsLayout="No",AND(OR(IsEnlarged="Yes",IsLayout="Yes"),properXrefFound="Yes")),"na","x"),IF(paperall&lt;3,"ok","x"))</f>
-        <v>na</v>
+        <f>IF(IsView="Yes",IF(OR(IsLayout="No",AND(OR(IsEnlarged="Yes",IsLayout="Yes"),properXrefFound="Yes")),"ok","x"),IF(paperall&lt;3,"ok","x"))</f>
+        <v>ok</v>
       </c>
       <c r="Q14" s="67"/>
       <c r="R14" s="67"/>
@@ -11379,7 +11389,7 @@
       <c r="DE14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF14" s="2" t="s">
+      <c r="DF14" s="138" t="s">
         <v>680</v>
       </c>
       <c r="DG14" s="2" t="s">
@@ -11683,7 +11693,7 @@
       <c r="DE15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF15" s="2" t="s">
+      <c r="DF15" s="138" t="s">
         <v>295</v>
       </c>
       <c r="DG15" s="2" t="s">
@@ -11970,7 +11980,7 @@
       <c r="DE16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF16" s="2" t="s">
+      <c r="DF16" s="138" t="s">
         <v>219</v>
       </c>
       <c r="DG16" s="2" t="s">
@@ -12196,7 +12206,7 @@
       <c r="DE17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF17" s="2" t="s">
+      <c r="DF17" s="138" t="s">
         <v>681</v>
       </c>
       <c r="DG17" s="2" t="s">
@@ -12415,7 +12425,7 @@
       <c r="DE18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF18" s="2" t="s">
+      <c r="DF18" s="138" t="s">
         <v>682</v>
       </c>
       <c r="DG18" s="2" t="s">
@@ -12480,7 +12490,7 @@
       </c>
       <c r="P19" s="37" t="str">
         <f>titleletter3</f>
-        <v>T</v>
+        <v>A</v>
       </c>
       <c r="Q19" s="37"/>
       <c r="R19" s="37" t="s">
@@ -12569,7 +12579,7 @@
       <c r="CD19" s="8"/>
       <c r="CE19" s="37"/>
       <c r="CF19" s="24" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="CG19" s="137">
         <v>7</v>
@@ -12624,7 +12634,7 @@
       <c r="DE19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DF19" s="2" t="s">
+      <c r="DF19" s="138" t="s">
         <v>209</v>
       </c>
       <c r="DG19" s="2" t="s">
@@ -12787,7 +12797,7 @@
         <v>47</v>
       </c>
       <c r="CG20" s="10" t="str">
-        <f>IF(IsView="Yes",IF(modelall=xrefsInModel,"ok","x"),IF(paperall&lt;3,"ok","x"))</f>
+        <f>IF(IsLayout="No","ok",IF(IsView="Yes",IF(modelall=xrefsInModel,"ok","x"),IF(paperall&lt;3,"ok","x")))</f>
         <v>ok</v>
       </c>
       <c r="CH20" s="38"/>
@@ -12830,7 +12840,7 @@
       </c>
       <c r="DD20" s="2"/>
       <c r="DE20" s="2"/>
-      <c r="DF20" s="2"/>
+      <c r="DF20" s="138"/>
       <c r="DG20" s="2"/>
       <c r="DH20" s="8"/>
       <c r="DK20" s="7"/>
@@ -12889,7 +12899,7 @@
       </c>
       <c r="P21" s="37" t="str">
         <f>titleletter5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="37"/>
       <c r="R21" s="37">
@@ -13014,7 +13024,7 @@
       </c>
       <c r="DD21" s="2"/>
       <c r="DE21" s="2"/>
-      <c r="DF21" s="2"/>
+      <c r="DF21" s="138"/>
       <c r="DG21" s="2"/>
       <c r="DH21" s="8"/>
       <c r="DK21" s="7"/>
@@ -13067,12 +13077,12 @@
       </c>
       <c r="P22" s="37" t="str">
         <f>titleletter6</f>
-        <v>2</v>
+        <v>-</v>
       </c>
       <c r="Q22" s="37"/>
       <c r="R22" s="37" t="str">
         <f>titleletter6</f>
-        <v>2</v>
+        <v>-</v>
       </c>
       <c r="S22" s="37"/>
       <c r="T22" s="37"/>
@@ -13193,7 +13203,7 @@
       </c>
       <c r="DD22" s="2"/>
       <c r="DE22" s="2"/>
-      <c r="DF22" s="2"/>
+      <c r="DF22" s="138"/>
       <c r="DG22" s="2"/>
       <c r="DH22" s="8"/>
       <c r="DK22" s="7"/>
@@ -13228,7 +13238,7 @@
       </c>
       <c r="E23" s="25" t="str">
         <f>MID($D$5,3,2)</f>
-        <v>T-</v>
+        <v>A-</v>
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
@@ -13250,7 +13260,7 @@
       <c r="Q23" s="37"/>
       <c r="R23" s="37" t="str">
         <f>titleletter7</f>
-        <v>2</v>
+        <v>O</v>
       </c>
       <c r="S23" s="37"/>
       <c r="T23" s="37"/>
@@ -13371,7 +13381,7 @@
       </c>
       <c r="DD23" s="2"/>
       <c r="DE23" s="2"/>
-      <c r="DF23" s="2"/>
+      <c r="DF23" s="138"/>
       <c r="DG23" s="2"/>
       <c r="DH23" s="8"/>
       <c r="DK23" s="7"/>
@@ -13406,7 +13416,7 @@
       </c>
       <c r="E24" s="25" t="str">
         <f>VLOOKUP(titleletters34,NCDisciplines,2,FALSE)</f>
-        <v xml:space="preserve">Telecommunications </v>
+        <v xml:space="preserve">Architectural </v>
       </c>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
@@ -13428,7 +13438,7 @@
       <c r="Q24" s="37"/>
       <c r="R24" s="37" t="str">
         <f>titleletter8</f>
-        <v>0</v>
+        <v>V</v>
       </c>
       <c r="S24" s="37"/>
       <c r="T24" s="37"/>
@@ -13549,7 +13559,7 @@
       </c>
       <c r="DD24" s="2"/>
       <c r="DE24" s="2"/>
-      <c r="DF24" s="2"/>
+      <c r="DF24" s="138"/>
       <c r="DG24" s="2"/>
       <c r="DH24" s="8"/>
       <c r="DK24" s="7"/>
@@ -13715,7 +13725,7 @@
       </c>
       <c r="DD25" s="2"/>
       <c r="DE25" s="2"/>
-      <c r="DF25" s="2"/>
+      <c r="DF25" s="138"/>
       <c r="DG25" s="2"/>
       <c r="DH25" s="8"/>
       <c r="DK25" s="7"/>
@@ -13750,7 +13760,7 @@
       </c>
       <c r="E26" s="25" t="str">
         <f>CONCATENATE(E7,MID($D$5,5,2))</f>
-        <v>S02</v>
+        <v>S1-</v>
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
@@ -13768,12 +13778,12 @@
       </c>
       <c r="P26" s="38" t="str">
         <f>CONCATENATE(P17,P18,P19,P20,P21,P22,P23,P24)</f>
-        <v>GST-02OV</v>
+        <v>GSA-1-OV</v>
       </c>
       <c r="Q26" s="38"/>
       <c r="R26" s="38" t="str">
         <f>CONCATENATE(R17,R18,R19,R20,R21,R22,R23,R24)</f>
-        <v>GSG-0220</v>
+        <v>GSG-0-OV</v>
       </c>
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
@@ -13891,7 +13901,7 @@
       </c>
       <c r="DD26" s="2"/>
       <c r="DE26" s="2"/>
-      <c r="DF26" s="2"/>
+      <c r="DF26" s="138"/>
       <c r="DG26" s="2"/>
       <c r="DH26" s="8"/>
       <c r="DK26" s="7"/>
@@ -13926,7 +13936,7 @@
       </c>
       <c r="E27" s="25" t="str">
         <f>IF(IsLayout="Yes",VLOOKUP(titleletters256,NCLevels,2,FALSE),"na")</f>
-        <v>na</v>
+        <v>Level 1 (Ground)</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -14038,7 +14048,7 @@
       </c>
       <c r="DD27" s="2"/>
       <c r="DE27" s="2"/>
-      <c r="DF27" s="2"/>
+      <c r="DF27" s="138"/>
       <c r="DG27" s="2"/>
       <c r="DH27" s="8"/>
       <c r="DK27" s="7"/>
@@ -14182,7 +14192,7 @@
       </c>
       <c r="DD28" s="2"/>
       <c r="DE28" s="2"/>
-      <c r="DF28" s="2"/>
+      <c r="DF28" s="138"/>
       <c r="DG28" s="2"/>
       <c r="DH28" s="8"/>
       <c r="DK28" s="7"/>
@@ -14217,7 +14227,7 @@
       </c>
       <c r="E29" s="25" t="str">
         <f>titleletter6</f>
-        <v>2</v>
+        <v>-</v>
       </c>
       <c r="F29" s="37"/>
       <c r="G29" s="37"/>
@@ -14329,7 +14339,7 @@
       </c>
       <c r="DD29" s="2"/>
       <c r="DE29" s="2"/>
-      <c r="DF29" s="2"/>
+      <c r="DF29" s="138"/>
       <c r="DG29" s="2"/>
       <c r="DH29" s="8"/>
       <c r="DK29" s="7"/>
@@ -14362,9 +14372,9 @@
       <c r="D30" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="E30" s="25" t="str">
+      <c r="E30" s="25" t="e">
         <f>IF(IsLayout="Yes",VLOOKUP(titleletter6,NCSpecial,2,FALSE),"na")</f>
-        <v>na</v>
+        <v>#N/A</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -14476,7 +14486,7 @@
       </c>
       <c r="DD30" s="2"/>
       <c r="DE30" s="2"/>
-      <c r="DF30" s="2"/>
+      <c r="DF30" s="138"/>
       <c r="DG30" s="2"/>
       <c r="DH30" s="8"/>
       <c r="DK30" s="7"/>
@@ -14618,7 +14628,7 @@
       </c>
       <c r="DD31" s="2"/>
       <c r="DE31" s="2"/>
-      <c r="DF31" s="2"/>
+      <c r="DF31" s="138"/>
       <c r="DG31" s="2"/>
       <c r="DH31" s="8"/>
       <c r="DK31" s="7"/>
@@ -14654,7 +14664,7 @@
       </c>
       <c r="E32" s="25" t="str">
         <f>MID($D$5,7,2)</f>
-        <v>20</v>
+        <v>OV</v>
       </c>
       <c r="F32" s="67"/>
       <c r="G32" s="67"/>
@@ -14789,7 +14799,7 @@
       </c>
       <c r="DD32" s="2"/>
       <c r="DE32" s="2"/>
-      <c r="DF32" s="2"/>
+      <c r="DF32" s="138"/>
       <c r="DG32" s="2"/>
       <c r="DH32" s="8"/>
       <c r="DK32" s="7"/>
@@ -14825,7 +14835,7 @@
       </c>
       <c r="E33" s="25" t="str">
         <f>IF(IsLayout="Yes",VLOOKUP(titleletter78,NCPlanKey,2,FALSE),"na")</f>
-        <v>na</v>
+        <v>Overview</v>
       </c>
       <c r="F33" s="67"/>
       <c r="G33" s="67"/>
@@ -14960,7 +14970,7 @@
       </c>
       <c r="DD33" s="2"/>
       <c r="DE33" s="2"/>
-      <c r="DF33" s="2"/>
+      <c r="DF33" s="138"/>
       <c r="DG33" s="2"/>
       <c r="DH33" s="8"/>
       <c r="DK33" s="7"/>
@@ -15102,7 +15112,7 @@
       </c>
       <c r="DD34" s="2"/>
       <c r="DE34" s="2"/>
-      <c r="DF34" s="2"/>
+      <c r="DF34" s="138"/>
       <c r="DG34" s="2"/>
       <c r="DH34" s="8"/>
       <c r="DK34" s="7"/>
@@ -15137,7 +15147,7 @@
       </c>
       <c r="E35" s="25" t="str">
         <f>MID($D$5,5,4)</f>
-        <v>0220</v>
+        <v>1-OV</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
@@ -15249,7 +15259,7 @@
       </c>
       <c r="DD35" s="2"/>
       <c r="DE35" s="2"/>
-      <c r="DF35" s="2"/>
+      <c r="DF35" s="138"/>
       <c r="DG35" s="2"/>
       <c r="DH35" s="8"/>
       <c r="DK35" s="7"/>
@@ -15284,7 +15294,7 @@
       </c>
       <c r="E36" s="27" t="str">
         <f>IF(IsLayout="No",VLOOKUP("Yes",NCSeries,4,FALSE),"na")</f>
-        <v>Diagrams and schematics (e.g. block, ladder, one-line and riser diagrams, PLC Communication), Electrical panel</v>
+        <v>na</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
@@ -15399,7 +15409,7 @@
       </c>
       <c r="DD36" s="2"/>
       <c r="DE36" s="2"/>
-      <c r="DF36" s="2"/>
+      <c r="DF36" s="138"/>
       <c r="DG36" s="2"/>
       <c r="DH36" s="8"/>
       <c r="DK36" s="7"/>
@@ -15544,7 +15554,7 @@
       </c>
       <c r="DD37" s="2"/>
       <c r="DE37" s="2"/>
-      <c r="DF37" s="2"/>
+      <c r="DF37" s="138"/>
       <c r="DG37" s="2"/>
       <c r="DH37" s="8"/>
       <c r="DK37" s="7"/>
@@ -15694,7 +15704,7 @@
       </c>
       <c r="DD38" s="2"/>
       <c r="DE38" s="2"/>
-      <c r="DF38" s="2"/>
+      <c r="DF38" s="138"/>
       <c r="DG38" s="2"/>
       <c r="DH38" s="8"/>
       <c r="DK38" s="7"/>
@@ -15839,7 +15849,7 @@
       </c>
       <c r="DD39" s="2"/>
       <c r="DE39" s="2"/>
-      <c r="DF39" s="2"/>
+      <c r="DF39" s="138"/>
       <c r="DG39" s="2"/>
       <c r="DH39" s="8"/>
       <c r="DK39" s="7"/>
@@ -15869,7 +15879,7 @@
       </c>
       <c r="E40" t="str">
         <f>IF(ISERROR(VLOOKUP(titleletter78,NCPlanKey,1,FALSE)),"No",IF(titleletter78=VLOOKUP(titleletter78,NCPlanKey,1,FALSE),"Yes","No"))</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
@@ -15984,7 +15994,7 @@
       </c>
       <c r="DD40" s="2"/>
       <c r="DE40" s="2"/>
-      <c r="DF40" s="2"/>
+      <c r="DF40" s="138"/>
       <c r="DG40" s="2"/>
       <c r="DH40" s="8"/>
       <c r="DK40" s="7"/>
@@ -16061,7 +16071,7 @@
       </c>
       <c r="DD41" s="2"/>
       <c r="DE41" s="2"/>
-      <c r="DF41" s="2"/>
+      <c r="DF41" s="138"/>
       <c r="DG41" s="2"/>
       <c r="DH41" s="8"/>
       <c r="DK41" s="7"/>
@@ -16133,7 +16143,7 @@
       </c>
       <c r="DD42" s="2"/>
       <c r="DE42" s="2"/>
-      <c r="DF42" s="2"/>
+      <c r="DF42" s="138"/>
       <c r="DG42" s="2"/>
       <c r="DH42" s="8"/>
       <c r="DK42" s="7"/>
@@ -16169,7 +16179,7 @@
       </c>
       <c r="K43" s="103" t="str">
         <f>IF(IsLayout="Yes",IF(layoutOrViewInTitle="Yes","Yes","No"),IF(title4WithKeyWord="Yes","Yes","No"))</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="L43" s="67"/>
       <c r="M43" s="25"/>
@@ -16234,7 +16244,7 @@
       </c>
       <c r="DD43" s="2"/>
       <c r="DE43" s="2"/>
-      <c r="DF43" s="2"/>
+      <c r="DF43" s="138"/>
       <c r="DG43" s="2"/>
       <c r="DH43" s="8"/>
       <c r="DK43" s="7"/>
@@ -16341,7 +16351,7 @@
       </c>
       <c r="DD44" s="2"/>
       <c r="DE44" s="2"/>
-      <c r="DF44" s="2"/>
+      <c r="DF44" s="138"/>
       <c r="DG44" s="2"/>
       <c r="DH44" s="8"/>
       <c r="DK44" s="7"/>
@@ -16442,7 +16452,7 @@
       </c>
       <c r="DD45" s="2"/>
       <c r="DE45" s="2"/>
-      <c r="DF45" s="2"/>
+      <c r="DF45" s="138"/>
       <c r="DG45" s="2"/>
       <c r="DH45" s="8"/>
       <c r="DK45" s="9"/>
@@ -16541,7 +16551,7 @@
       </c>
       <c r="DD46" s="2"/>
       <c r="DE46" s="2"/>
-      <c r="DF46" s="2"/>
+      <c r="DF46" s="138"/>
       <c r="DG46" s="2"/>
       <c r="DH46" s="8"/>
     </row>
@@ -16563,7 +16573,7 @@
       </c>
       <c r="K47" s="4" t="str">
         <f>IF(AND(IsLayout="No",M14="Yes"),"ok",  IF(IsView="Yes",IF(AND(titleinmodel="No",titleinpaper="Yes",UniqueTitle="Yes",title4proper="Yes",title3proper="Yes",title2proper="Yes",title1proper="Yes",scaleformatok="Yes",plotscaleok="Yes"),"ok","x"),"na"))</f>
-        <v>ok</v>
+        <v>x</v>
       </c>
       <c r="L47" s="37"/>
       <c r="M47" s="25"/>
@@ -16623,7 +16633,7 @@
       </c>
       <c r="DD47" s="2"/>
       <c r="DE47" s="2"/>
-      <c r="DF47" s="2"/>
+      <c r="DF47" s="138"/>
       <c r="DG47" s="2"/>
       <c r="DH47" s="8"/>
     </row>
@@ -16634,7 +16644,7 @@
       </c>
       <c r="E48" s="38" t="str">
         <f>'chk1'!H60</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="F48" s="82"/>
       <c r="G48" s="82"/>
@@ -16700,7 +16710,7 @@
       </c>
       <c r="DD48" s="2"/>
       <c r="DE48" s="2"/>
-      <c r="DF48" s="2"/>
+      <c r="DF48" s="138"/>
       <c r="DG48" s="2"/>
       <c r="DH48" s="8"/>
     </row>
@@ -16768,7 +16778,7 @@
       </c>
       <c r="DD49" s="2"/>
       <c r="DE49" s="2"/>
-      <c r="DF49" s="2"/>
+      <c r="DF49" s="138"/>
       <c r="DG49" s="2"/>
       <c r="DH49" s="8"/>
     </row>
@@ -16836,7 +16846,7 @@
       </c>
       <c r="DD50" s="2"/>
       <c r="DE50" s="2"/>
-      <c r="DF50" s="2"/>
+      <c r="DF50" s="138"/>
       <c r="DG50" s="2"/>
       <c r="DH50" s="8"/>
     </row>
@@ -16870,7 +16880,7 @@
       </c>
       <c r="DD51" s="2"/>
       <c r="DE51" s="2"/>
-      <c r="DF51" s="2"/>
+      <c r="DF51" s="138"/>
       <c r="DG51" s="2"/>
       <c r="DH51" s="8"/>
     </row>
@@ -16903,7 +16913,7 @@
       </c>
       <c r="DD52" s="2"/>
       <c r="DE52" s="2"/>
-      <c r="DF52" s="2"/>
+      <c r="DF52" s="138"/>
       <c r="DG52" s="2"/>
       <c r="DH52" s="8"/>
     </row>
@@ -16936,7 +16946,7 @@
       </c>
       <c r="DD53" s="2"/>
       <c r="DE53" s="2"/>
-      <c r="DF53" s="2"/>
+      <c r="DF53" s="138"/>
       <c r="DG53" s="2"/>
       <c r="DH53" s="8"/>
     </row>
@@ -16969,7 +16979,7 @@
       </c>
       <c r="DD54" s="2"/>
       <c r="DE54" s="2"/>
-      <c r="DF54" s="2"/>
+      <c r="DF54" s="138"/>
       <c r="DG54" s="2"/>
       <c r="DH54" s="8"/>
     </row>
@@ -17002,7 +17012,7 @@
       </c>
       <c r="DD55" s="2"/>
       <c r="DE55" s="2"/>
-      <c r="DF55" s="2"/>
+      <c r="DF55" s="138"/>
       <c r="DG55" s="2"/>
       <c r="DH55" s="8"/>
     </row>
@@ -17035,7 +17045,7 @@
       </c>
       <c r="DD56" s="2"/>
       <c r="DE56" s="2"/>
-      <c r="DF56" s="2"/>
+      <c r="DF56" s="138"/>
       <c r="DG56" s="2"/>
       <c r="DH56" s="8"/>
     </row>
@@ -17068,7 +17078,7 @@
       </c>
       <c r="DD57" s="2"/>
       <c r="DE57" s="2"/>
-      <c r="DF57" s="2"/>
+      <c r="DF57" s="138"/>
       <c r="DG57" s="2"/>
       <c r="DH57" s="8"/>
     </row>
@@ -17101,7 +17111,7 @@
       </c>
       <c r="DD58" s="2"/>
       <c r="DE58" s="2"/>
-      <c r="DF58" s="2"/>
+      <c r="DF58" s="138"/>
       <c r="DG58" s="2"/>
       <c r="DH58" s="8"/>
     </row>
@@ -17134,7 +17144,7 @@
       </c>
       <c r="DD59" s="2"/>
       <c r="DE59" s="2"/>
-      <c r="DF59" s="2"/>
+      <c r="DF59" s="138"/>
       <c r="DG59" s="2"/>
       <c r="DH59" s="8"/>
     </row>
@@ -17167,7 +17177,7 @@
       </c>
       <c r="DD60" s="2"/>
       <c r="DE60" s="2"/>
-      <c r="DF60" s="2"/>
+      <c r="DF60" s="138"/>
       <c r="DG60" s="2"/>
       <c r="DH60" s="8"/>
     </row>
@@ -17200,7 +17210,7 @@
       </c>
       <c r="DD61" s="2"/>
       <c r="DE61" s="2"/>
-      <c r="DF61" s="2"/>
+      <c r="DF61" s="138"/>
       <c r="DG61" s="2"/>
       <c r="DH61" s="8"/>
     </row>
@@ -17240,7 +17250,7 @@
       </c>
       <c r="DD62" s="2"/>
       <c r="DE62" s="2"/>
-      <c r="DF62" s="2"/>
+      <c r="DF62" s="138"/>
       <c r="DG62" s="2"/>
       <c r="DH62" s="8"/>
     </row>
@@ -17273,7 +17283,7 @@
       </c>
       <c r="DD63" s="2"/>
       <c r="DE63" s="2"/>
-      <c r="DF63" s="2"/>
+      <c r="DF63" s="138"/>
       <c r="DG63" s="2"/>
       <c r="DH63" s="8"/>
     </row>
@@ -17306,7 +17316,7 @@
       </c>
       <c r="DD64" s="2"/>
       <c r="DE64" s="2"/>
-      <c r="DF64" s="2"/>
+      <c r="DF64" s="138"/>
       <c r="DG64" s="2"/>
       <c r="DH64" s="8"/>
     </row>
@@ -17339,7 +17349,7 @@
       </c>
       <c r="DD65" s="2"/>
       <c r="DE65" s="2"/>
-      <c r="DF65" s="2"/>
+      <c r="DF65" s="138"/>
       <c r="DG65" s="2"/>
       <c r="DH65" s="8"/>
     </row>
@@ -17372,7 +17382,7 @@
       </c>
       <c r="DD66" s="2"/>
       <c r="DE66" s="2"/>
-      <c r="DF66" s="2"/>
+      <c r="DF66" s="138"/>
       <c r="DG66" s="2"/>
       <c r="DH66" s="8"/>
     </row>
@@ -17405,7 +17415,7 @@
       </c>
       <c r="DD67" s="2"/>
       <c r="DE67" s="2"/>
-      <c r="DF67" s="2"/>
+      <c r="DF67" s="138"/>
       <c r="DG67" s="2"/>
       <c r="DH67" s="8"/>
     </row>
@@ -17438,7 +17448,7 @@
       </c>
       <c r="DD68" s="2"/>
       <c r="DE68" s="2"/>
-      <c r="DF68" s="2"/>
+      <c r="DF68" s="138"/>
       <c r="DG68" s="2"/>
       <c r="DH68" s="8"/>
     </row>
@@ -17471,7 +17481,7 @@
       </c>
       <c r="DD69" s="2"/>
       <c r="DE69" s="2"/>
-      <c r="DF69" s="2"/>
+      <c r="DF69" s="138"/>
       <c r="DG69" s="2"/>
       <c r="DH69" s="8"/>
     </row>
@@ -17504,7 +17514,7 @@
       </c>
       <c r="DD70" s="2"/>
       <c r="DE70" s="2"/>
-      <c r="DF70" s="2"/>
+      <c r="DF70" s="138"/>
       <c r="DG70" s="2"/>
       <c r="DH70" s="8"/>
     </row>
@@ -17537,7 +17547,7 @@
       </c>
       <c r="DD71" s="2"/>
       <c r="DE71" s="2"/>
-      <c r="DF71" s="2"/>
+      <c r="DF71" s="138"/>
       <c r="DG71" s="2"/>
       <c r="DH71" s="8"/>
     </row>
@@ -17570,7 +17580,7 @@
       </c>
       <c r="DD72" s="2"/>
       <c r="DE72" s="2"/>
-      <c r="DF72" s="2"/>
+      <c r="DF72" s="138"/>
       <c r="DG72" s="2"/>
       <c r="DH72" s="8"/>
     </row>
@@ -17603,7 +17613,7 @@
       </c>
       <c r="DD73" s="2"/>
       <c r="DE73" s="2"/>
-      <c r="DF73" s="2"/>
+      <c r="DF73" s="138"/>
       <c r="DG73" s="2"/>
       <c r="DH73" s="8"/>
     </row>
@@ -17636,7 +17646,7 @@
       </c>
       <c r="DD74" s="2"/>
       <c r="DE74" s="2"/>
-      <c r="DF74" s="2"/>
+      <c r="DF74" s="138"/>
       <c r="DG74" s="2"/>
       <c r="DH74" s="8"/>
     </row>
@@ -17669,7 +17679,7 @@
       </c>
       <c r="DD75" s="2"/>
       <c r="DE75" s="2"/>
-      <c r="DF75" s="2"/>
+      <c r="DF75" s="138"/>
       <c r="DG75" s="2"/>
       <c r="DH75" s="8"/>
     </row>
@@ -17702,7 +17712,7 @@
       </c>
       <c r="DD76" s="2"/>
       <c r="DE76" s="2"/>
-      <c r="DF76" s="2"/>
+      <c r="DF76" s="138"/>
       <c r="DG76" s="2"/>
       <c r="DH76" s="8"/>
     </row>
@@ -17735,7 +17745,7 @@
       </c>
       <c r="DD77" s="2"/>
       <c r="DE77" s="2"/>
-      <c r="DF77" s="2"/>
+      <c r="DF77" s="138"/>
       <c r="DG77" s="2"/>
       <c r="DH77" s="8"/>
     </row>
@@ -17768,7 +17778,7 @@
       </c>
       <c r="DD78" s="2"/>
       <c r="DE78" s="2"/>
-      <c r="DF78" s="2"/>
+      <c r="DF78" s="138"/>
       <c r="DG78" s="2"/>
       <c r="DH78" s="8"/>
     </row>
@@ -17801,7 +17811,7 @@
       </c>
       <c r="DD79" s="2"/>
       <c r="DE79" s="2"/>
-      <c r="DF79" s="2"/>
+      <c r="DF79" s="138"/>
       <c r="DG79" s="2"/>
       <c r="DH79" s="8"/>
     </row>
@@ -17834,7 +17844,7 @@
       </c>
       <c r="DD80" s="2"/>
       <c r="DE80" s="2"/>
-      <c r="DF80" s="2"/>
+      <c r="DF80" s="138"/>
       <c r="DG80" s="2"/>
       <c r="DH80" s="8"/>
     </row>
@@ -17867,7 +17877,7 @@
       </c>
       <c r="DD81" s="2"/>
       <c r="DE81" s="2"/>
-      <c r="DF81" s="2"/>
+      <c r="DF81" s="138"/>
       <c r="DG81" s="2"/>
       <c r="DH81" s="8"/>
     </row>
@@ -17900,7 +17910,7 @@
       </c>
       <c r="DD82" s="2"/>
       <c r="DE82" s="2"/>
-      <c r="DF82" s="2"/>
+      <c r="DF82" s="138"/>
       <c r="DG82" s="2"/>
       <c r="DH82" s="8"/>
     </row>
@@ -17933,7 +17943,7 @@
       </c>
       <c r="DD83" s="2"/>
       <c r="DE83" s="2"/>
-      <c r="DF83" s="2"/>
+      <c r="DF83" s="138"/>
       <c r="DG83" s="2"/>
       <c r="DH83" s="8"/>
     </row>
@@ -17966,7 +17976,7 @@
       </c>
       <c r="DD84" s="2"/>
       <c r="DE84" s="2"/>
-      <c r="DF84" s="2"/>
+      <c r="DF84" s="138"/>
       <c r="DG84" s="2"/>
       <c r="DH84" s="8"/>
     </row>
@@ -17999,7 +18009,7 @@
       </c>
       <c r="DD85" s="2"/>
       <c r="DE85" s="2"/>
-      <c r="DF85" s="2"/>
+      <c r="DF85" s="138"/>
       <c r="DG85" s="2"/>
       <c r="DH85" s="8"/>
     </row>
@@ -18032,7 +18042,7 @@
       </c>
       <c r="DD86" s="2"/>
       <c r="DE86" s="2"/>
-      <c r="DF86" s="2"/>
+      <c r="DF86" s="138"/>
       <c r="DG86" s="2"/>
       <c r="DH86" s="8"/>
     </row>
@@ -18065,7 +18075,7 @@
       </c>
       <c r="DD87" s="2"/>
       <c r="DE87" s="2"/>
-      <c r="DF87" s="2"/>
+      <c r="DF87" s="138"/>
       <c r="DG87" s="2"/>
       <c r="DH87" s="8"/>
     </row>
@@ -18098,7 +18108,7 @@
       </c>
       <c r="DD88" s="2"/>
       <c r="DE88" s="2"/>
-      <c r="DF88" s="2"/>
+      <c r="DF88" s="138"/>
       <c r="DG88" s="2"/>
       <c r="DH88" s="8"/>
     </row>
@@ -18131,7 +18141,7 @@
       </c>
       <c r="DD89" s="2"/>
       <c r="DE89" s="2"/>
-      <c r="DF89" s="2"/>
+      <c r="DF89" s="138"/>
       <c r="DG89" s="2"/>
       <c r="DH89" s="8"/>
     </row>
@@ -18164,7 +18174,7 @@
       </c>
       <c r="DD90" s="2"/>
       <c r="DE90" s="2"/>
-      <c r="DF90" s="2"/>
+      <c r="DF90" s="138"/>
       <c r="DG90" s="2"/>
       <c r="DH90" s="8"/>
     </row>
@@ -18197,7 +18207,7 @@
       </c>
       <c r="DD91" s="2"/>
       <c r="DE91" s="2"/>
-      <c r="DF91" s="2"/>
+      <c r="DF91" s="138"/>
       <c r="DG91" s="2"/>
       <c r="DH91" s="8"/>
     </row>
@@ -18230,7 +18240,7 @@
       </c>
       <c r="DD92" s="2"/>
       <c r="DE92" s="2"/>
-      <c r="DF92" s="2"/>
+      <c r="DF92" s="138"/>
       <c r="DG92" s="2"/>
       <c r="DH92" s="8"/>
     </row>
@@ -18263,7 +18273,7 @@
       </c>
       <c r="DD93" s="2"/>
       <c r="DE93" s="2"/>
-      <c r="DF93" s="2"/>
+      <c r="DF93" s="138"/>
       <c r="DG93" s="2"/>
       <c r="DH93" s="8"/>
     </row>
@@ -18296,7 +18306,7 @@
       </c>
       <c r="DD94" s="2"/>
       <c r="DE94" s="2"/>
-      <c r="DF94" s="2"/>
+      <c r="DF94" s="138"/>
       <c r="DG94" s="2"/>
       <c r="DH94" s="8"/>
     </row>
@@ -18329,7 +18339,7 @@
       </c>
       <c r="DD95" s="2"/>
       <c r="DE95" s="2"/>
-      <c r="DF95" s="2"/>
+      <c r="DF95" s="138"/>
       <c r="DG95" s="2"/>
       <c r="DH95" s="8"/>
     </row>
@@ -18362,7 +18372,7 @@
       </c>
       <c r="DD96" s="2"/>
       <c r="DE96" s="2"/>
-      <c r="DF96" s="2"/>
+      <c r="DF96" s="138"/>
       <c r="DG96" s="2"/>
       <c r="DH96" s="8"/>
     </row>
@@ -18395,7 +18405,7 @@
       </c>
       <c r="DD97" s="2"/>
       <c r="DE97" s="2"/>
-      <c r="DF97" s="2"/>
+      <c r="DF97" s="138"/>
       <c r="DG97" s="2"/>
       <c r="DH97" s="8"/>
     </row>
@@ -18428,7 +18438,7 @@
       </c>
       <c r="DD98" s="2"/>
       <c r="DE98" s="2"/>
-      <c r="DF98" s="2"/>
+      <c r="DF98" s="138"/>
       <c r="DG98" s="2"/>
       <c r="DH98" s="8"/>
     </row>
@@ -18461,7 +18471,7 @@
       </c>
       <c r="DD99" s="2"/>
       <c r="DE99" s="2"/>
-      <c r="DF99" s="2"/>
+      <c r="DF99" s="138"/>
       <c r="DG99" s="2"/>
       <c r="DH99" s="8"/>
     </row>
@@ -18494,7 +18504,7 @@
       </c>
       <c r="DD100" s="2"/>
       <c r="DE100" s="2"/>
-      <c r="DF100" s="2"/>
+      <c r="DF100" s="138"/>
       <c r="DG100" s="2"/>
       <c r="DH100" s="8"/>
     </row>
@@ -18527,7 +18537,7 @@
       </c>
       <c r="DD101" s="2"/>
       <c r="DE101" s="2"/>
-      <c r="DF101" s="2"/>
+      <c r="DF101" s="138"/>
       <c r="DG101" s="2"/>
       <c r="DH101" s="8"/>
     </row>
@@ -18560,7 +18570,7 @@
       </c>
       <c r="DD102" s="2"/>
       <c r="DE102" s="2"/>
-      <c r="DF102" s="2"/>
+      <c r="DF102" s="138"/>
       <c r="DG102" s="2"/>
       <c r="DH102" s="8"/>
     </row>
@@ -18593,7 +18603,7 @@
       </c>
       <c r="DD103" s="2"/>
       <c r="DE103" s="2"/>
-      <c r="DF103" s="2"/>
+      <c r="DF103" s="138"/>
       <c r="DG103" s="2"/>
       <c r="DH103" s="8"/>
     </row>
@@ -18626,7 +18636,7 @@
       </c>
       <c r="DD104" s="2"/>
       <c r="DE104" s="2"/>
-      <c r="DF104" s="2"/>
+      <c r="DF104" s="138"/>
       <c r="DG104" s="2"/>
       <c r="DH104" s="8"/>
     </row>
@@ -18659,7 +18669,7 @@
       </c>
       <c r="DD105" s="2"/>
       <c r="DE105" s="2"/>
-      <c r="DF105" s="2"/>
+      <c r="DF105" s="138"/>
       <c r="DG105" s="2"/>
       <c r="DH105" s="8"/>
     </row>
@@ -18692,7 +18702,7 @@
       </c>
       <c r="DD106" s="2"/>
       <c r="DE106" s="2"/>
-      <c r="DF106" s="2"/>
+      <c r="DF106" s="138"/>
       <c r="DG106" s="2"/>
       <c r="DH106" s="8"/>
     </row>
@@ -18725,7 +18735,7 @@
       </c>
       <c r="DD107" s="2"/>
       <c r="DE107" s="2"/>
-      <c r="DF107" s="2"/>
+      <c r="DF107" s="138"/>
       <c r="DG107" s="2"/>
       <c r="DH107" s="8"/>
     </row>
@@ -18758,7 +18768,7 @@
       </c>
       <c r="DD108" s="2"/>
       <c r="DE108" s="2"/>
-      <c r="DF108" s="2"/>
+      <c r="DF108" s="138"/>
       <c r="DG108" s="2"/>
       <c r="DH108" s="8"/>
     </row>
@@ -18791,7 +18801,7 @@
       </c>
       <c r="DD109" s="2"/>
       <c r="DE109" s="2"/>
-      <c r="DF109" s="2"/>
+      <c r="DF109" s="138"/>
       <c r="DG109" s="2"/>
       <c r="DH109" s="8"/>
     </row>
@@ -18824,7 +18834,7 @@
       </c>
       <c r="DD110" s="2"/>
       <c r="DE110" s="2"/>
-      <c r="DF110" s="2"/>
+      <c r="DF110" s="138"/>
       <c r="DG110" s="2"/>
       <c r="DH110" s="8"/>
     </row>
@@ -18857,7 +18867,7 @@
       </c>
       <c r="DD111" s="2"/>
       <c r="DE111" s="2"/>
-      <c r="DF111" s="2"/>
+      <c r="DF111" s="138"/>
       <c r="DG111" s="2"/>
       <c r="DH111" s="8"/>
     </row>
@@ -18890,7 +18900,7 @@
       </c>
       <c r="DD112" s="2"/>
       <c r="DE112" s="2"/>
-      <c r="DF112" s="2"/>
+      <c r="DF112" s="138"/>
       <c r="DG112" s="2"/>
       <c r="DH112" s="8"/>
     </row>
@@ -18923,7 +18933,7 @@
       </c>
       <c r="DD113" s="2"/>
       <c r="DE113" s="2"/>
-      <c r="DF113" s="2"/>
+      <c r="DF113" s="138"/>
       <c r="DG113" s="2"/>
       <c r="DH113" s="8"/>
     </row>
@@ -18956,7 +18966,7 @@
       </c>
       <c r="DD114" s="2"/>
       <c r="DE114" s="2"/>
-      <c r="DF114" s="2"/>
+      <c r="DF114" s="138"/>
       <c r="DG114" s="2"/>
       <c r="DH114" s="8"/>
     </row>
@@ -18989,7 +18999,7 @@
       </c>
       <c r="DD115" s="2"/>
       <c r="DE115" s="2"/>
-      <c r="DF115" s="2"/>
+      <c r="DF115" s="138"/>
       <c r="DG115" s="2"/>
       <c r="DH115" s="8"/>
     </row>
@@ -19022,7 +19032,7 @@
       </c>
       <c r="DD116" s="2"/>
       <c r="DE116" s="2"/>
-      <c r="DF116" s="2"/>
+      <c r="DF116" s="138"/>
       <c r="DG116" s="2"/>
       <c r="DH116" s="8"/>
     </row>
@@ -19055,7 +19065,7 @@
       </c>
       <c r="DD117" s="2"/>
       <c r="DE117" s="2"/>
-      <c r="DF117" s="2"/>
+      <c r="DF117" s="138"/>
       <c r="DG117" s="2"/>
       <c r="DH117" s="8"/>
     </row>
@@ -19088,7 +19098,7 @@
       </c>
       <c r="DD118" s="2"/>
       <c r="DE118" s="2"/>
-      <c r="DF118" s="2"/>
+      <c r="DF118" s="138"/>
       <c r="DG118" s="2"/>
       <c r="DH118" s="8"/>
     </row>
@@ -19121,7 +19131,7 @@
       </c>
       <c r="DD119" s="2"/>
       <c r="DE119" s="2"/>
-      <c r="DF119" s="2"/>
+      <c r="DF119" s="138"/>
       <c r="DG119" s="2"/>
       <c r="DH119" s="8"/>
     </row>
@@ -19154,7 +19164,7 @@
       </c>
       <c r="DD120" s="2"/>
       <c r="DE120" s="2"/>
-      <c r="DF120" s="2"/>
+      <c r="DF120" s="138"/>
       <c r="DG120" s="2"/>
       <c r="DH120" s="8"/>
     </row>
@@ -19187,7 +19197,7 @@
       </c>
       <c r="DD121" s="2"/>
       <c r="DE121" s="2"/>
-      <c r="DF121" s="2"/>
+      <c r="DF121" s="138"/>
       <c r="DG121" s="2"/>
       <c r="DH121" s="8"/>
     </row>
@@ -19220,7 +19230,7 @@
       </c>
       <c r="DD122" s="2"/>
       <c r="DE122" s="2"/>
-      <c r="DF122" s="2"/>
+      <c r="DF122" s="138"/>
       <c r="DG122" s="2"/>
       <c r="DH122" s="8"/>
     </row>
@@ -19253,7 +19263,7 @@
       </c>
       <c r="DD123" s="2"/>
       <c r="DE123" s="2"/>
-      <c r="DF123" s="2"/>
+      <c r="DF123" s="138"/>
       <c r="DG123" s="2"/>
       <c r="DH123" s="8"/>
     </row>
@@ -19286,7 +19296,7 @@
       </c>
       <c r="DD124" s="2"/>
       <c r="DE124" s="2"/>
-      <c r="DF124" s="2"/>
+      <c r="DF124" s="138"/>
       <c r="DG124" s="2"/>
       <c r="DH124" s="8"/>
     </row>
@@ -19319,7 +19329,7 @@
       </c>
       <c r="DD125" s="2"/>
       <c r="DE125" s="2"/>
-      <c r="DF125" s="2"/>
+      <c r="DF125" s="138"/>
       <c r="DG125" s="2"/>
       <c r="DH125" s="8"/>
     </row>
@@ -19352,7 +19362,7 @@
       </c>
       <c r="DD126" s="2"/>
       <c r="DE126" s="2"/>
-      <c r="DF126" s="2"/>
+      <c r="DF126" s="138"/>
       <c r="DG126" s="2"/>
       <c r="DH126" s="8"/>
     </row>
@@ -19385,7 +19395,7 @@
       </c>
       <c r="DD127" s="2"/>
       <c r="DE127" s="2"/>
-      <c r="DF127" s="2"/>
+      <c r="DF127" s="138"/>
       <c r="DG127" s="2"/>
       <c r="DH127" s="8"/>
     </row>
@@ -19418,7 +19428,7 @@
       </c>
       <c r="DD128" s="2"/>
       <c r="DE128" s="2"/>
-      <c r="DF128" s="2"/>
+      <c r="DF128" s="138"/>
       <c r="DG128" s="2"/>
       <c r="DH128" s="8"/>
     </row>
@@ -19451,7 +19461,7 @@
       </c>
       <c r="DD129" s="2"/>
       <c r="DE129" s="2"/>
-      <c r="DF129" s="2"/>
+      <c r="DF129" s="138"/>
       <c r="DG129" s="2"/>
       <c r="DH129" s="8"/>
     </row>
@@ -19484,7 +19494,7 @@
       </c>
       <c r="DD130" s="2"/>
       <c r="DE130" s="2"/>
-      <c r="DF130" s="2"/>
+      <c r="DF130" s="138"/>
       <c r="DG130" s="2"/>
       <c r="DH130" s="8"/>
     </row>
@@ -19517,7 +19527,7 @@
       </c>
       <c r="DD131" s="2"/>
       <c r="DE131" s="2"/>
-      <c r="DF131" s="2"/>
+      <c r="DF131" s="138"/>
       <c r="DG131" s="2"/>
       <c r="DH131" s="8"/>
     </row>
@@ -19550,7 +19560,7 @@
       </c>
       <c r="DD132" s="2"/>
       <c r="DE132" s="2"/>
-      <c r="DF132" s="2"/>
+      <c r="DF132" s="138"/>
       <c r="DG132" s="2"/>
       <c r="DH132" s="8"/>
     </row>
@@ -19583,7 +19593,7 @@
       </c>
       <c r="DD133" s="2"/>
       <c r="DE133" s="2"/>
-      <c r="DF133" s="2"/>
+      <c r="DF133" s="138"/>
       <c r="DG133" s="2"/>
       <c r="DH133" s="8"/>
     </row>
@@ -19616,7 +19626,7 @@
       </c>
       <c r="DD134" s="2"/>
       <c r="DE134" s="2"/>
-      <c r="DF134" s="2"/>
+      <c r="DF134" s="138"/>
       <c r="DG134" s="2"/>
       <c r="DH134" s="8"/>
     </row>
@@ -19649,7 +19659,7 @@
       </c>
       <c r="DD135" s="2"/>
       <c r="DE135" s="2"/>
-      <c r="DF135" s="2"/>
+      <c r="DF135" s="138"/>
       <c r="DG135" s="2"/>
       <c r="DH135" s="8"/>
     </row>
@@ -19682,7 +19692,7 @@
       </c>
       <c r="DD136" s="2"/>
       <c r="DE136" s="2"/>
-      <c r="DF136" s="2"/>
+      <c r="DF136" s="138"/>
       <c r="DG136" s="2"/>
       <c r="DH136" s="8"/>
     </row>
@@ -19715,7 +19725,7 @@
       </c>
       <c r="DD137" s="2"/>
       <c r="DE137" s="2"/>
-      <c r="DF137" s="2"/>
+      <c r="DF137" s="138"/>
       <c r="DG137" s="2"/>
       <c r="DH137" s="8"/>
     </row>
@@ -19748,7 +19758,7 @@
       </c>
       <c r="DD138" s="2"/>
       <c r="DE138" s="2"/>
-      <c r="DF138" s="2"/>
+      <c r="DF138" s="138"/>
       <c r="DG138" s="2"/>
       <c r="DH138" s="8"/>
     </row>
@@ -19781,7 +19791,7 @@
       </c>
       <c r="DD139" s="2"/>
       <c r="DE139" s="2"/>
-      <c r="DF139" s="2"/>
+      <c r="DF139" s="138"/>
       <c r="DG139" s="2"/>
       <c r="DH139" s="8"/>
     </row>
@@ -19814,7 +19824,7 @@
       </c>
       <c r="DD140" s="2"/>
       <c r="DE140" s="2"/>
-      <c r="DF140" s="2"/>
+      <c r="DF140" s="138"/>
       <c r="DG140" s="2"/>
       <c r="DH140" s="8"/>
     </row>
@@ -19847,7 +19857,7 @@
       </c>
       <c r="DD141" s="2"/>
       <c r="DE141" s="2"/>
-      <c r="DF141" s="2"/>
+      <c r="DF141" s="138"/>
       <c r="DG141" s="2"/>
       <c r="DH141" s="8"/>
     </row>
@@ -19880,7 +19890,7 @@
       </c>
       <c r="DD142" s="2"/>
       <c r="DE142" s="2"/>
-      <c r="DF142" s="2"/>
+      <c r="DF142" s="138"/>
       <c r="DG142" s="2"/>
       <c r="DH142" s="8"/>
     </row>
@@ -19913,7 +19923,7 @@
       </c>
       <c r="DD143" s="2"/>
       <c r="DE143" s="2"/>
-      <c r="DF143" s="2"/>
+      <c r="DF143" s="138"/>
       <c r="DG143" s="2"/>
       <c r="DH143" s="8"/>
     </row>
@@ -19946,7 +19956,7 @@
       </c>
       <c r="DD144" s="2"/>
       <c r="DE144" s="2"/>
-      <c r="DF144" s="2"/>
+      <c r="DF144" s="138"/>
       <c r="DG144" s="2"/>
       <c r="DH144" s="8"/>
     </row>
@@ -19979,7 +19989,7 @@
       </c>
       <c r="DD145" s="2"/>
       <c r="DE145" s="2"/>
-      <c r="DF145" s="2"/>
+      <c r="DF145" s="138"/>
       <c r="DG145" s="2"/>
       <c r="DH145" s="8"/>
     </row>
@@ -20012,7 +20022,7 @@
       </c>
       <c r="DD146" s="2"/>
       <c r="DE146" s="2"/>
-      <c r="DF146" s="2"/>
+      <c r="DF146" s="138"/>
       <c r="DG146" s="2"/>
       <c r="DH146" s="8"/>
     </row>
@@ -20045,7 +20055,7 @@
       </c>
       <c r="DD147" s="2"/>
       <c r="DE147" s="2"/>
-      <c r="DF147" s="2"/>
+      <c r="DF147" s="138"/>
       <c r="DG147" s="2"/>
       <c r="DH147" s="8"/>
     </row>
@@ -20078,7 +20088,7 @@
       </c>
       <c r="DD148" s="2"/>
       <c r="DE148" s="2"/>
-      <c r="DF148" s="2"/>
+      <c r="DF148" s="138"/>
       <c r="DG148" s="2"/>
       <c r="DH148" s="8"/>
     </row>
@@ -20111,7 +20121,7 @@
       </c>
       <c r="DD149" s="2"/>
       <c r="DE149" s="2"/>
-      <c r="DF149" s="2"/>
+      <c r="DF149" s="138"/>
       <c r="DG149" s="2"/>
       <c r="DH149" s="8"/>
     </row>
@@ -20144,7 +20154,7 @@
       </c>
       <c r="DD150" s="10"/>
       <c r="DE150" s="10"/>
-      <c r="DF150" s="10"/>
+      <c r="DF150" s="165"/>
       <c r="DG150" s="10"/>
       <c r="DH150" s="11"/>
     </row>
@@ -21448,13 +21458,13 @@
       </c>
       <c r="H45" s="7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="L45" s="2">
         <v>200</v>
@@ -21488,7 +21498,7 @@
       </c>
       <c r="U45" s="122">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W45" s="7" t="s">
         <v>416</v>
@@ -22210,7 +22220,7 @@
       </c>
       <c r="H60" s="9" t="str">
         <f t="shared" ref="H60:I60" si="8">IF(SUM(H43:H58)&gt;0,"Yes","No")</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I60" s="10" t="str">
         <f t="shared" si="8"/>
@@ -22222,7 +22232,7 @@
       </c>
       <c r="U60" s="116" t="str">
         <f>IF(SUM(U43:U58)&gt;0,"Yes","No")</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="61" spans="4:25">

</xml_diff>